<commit_message>
modified crawler.extract_params() for all geometries
</commit_message>
<xml_diff>
--- a/project_overview.xlsx
+++ b/project_overview.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="Export Summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -3926,7 +3926,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>205920</xdr:colOff>
+      <xdr:colOff>205560</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>31680</xdr:rowOff>
     </xdr:to>
@@ -3938,7 +3938,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="3027600" cy="526680"/>
+          <a:ext cx="3027240" cy="526680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3991,7 +3991,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>205920</xdr:colOff>
+      <xdr:colOff>205560</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>15120</xdr:rowOff>
     </xdr:to>
@@ -4003,7 +4003,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="7247880"/>
-          <a:ext cx="3027600" cy="526680"/>
+          <a:ext cx="3027240" cy="526680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4061,7 +4061,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>42840</xdr:colOff>
+      <xdr:colOff>42480</xdr:colOff>
       <xdr:row>108</xdr:row>
       <xdr:rowOff>75960</xdr:rowOff>
     </xdr:to>
@@ -4073,7 +4073,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="60120" y="16951680"/>
-          <a:ext cx="6332040" cy="952200"/>
+          <a:ext cx="6331680" cy="952200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4126,7 +4126,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>89640</xdr:colOff>
+      <xdr:colOff>89280</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>129240</xdr:rowOff>
     </xdr:to>
@@ -4138,7 +4138,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="60120" y="0"/>
-          <a:ext cx="7084080" cy="952200"/>
+          <a:ext cx="7083720" cy="952200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4196,7 +4196,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>258480</xdr:colOff>
+      <xdr:colOff>258120</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>126720</xdr:rowOff>
     </xdr:to>
@@ -4208,7 +4208,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="4491360" cy="952200"/>
+          <a:ext cx="4491000" cy="952200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4261,7 +4261,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>258480</xdr:colOff>
+      <xdr:colOff>258120</xdr:colOff>
       <xdr:row>114</xdr:row>
       <xdr:rowOff>160200</xdr:rowOff>
     </xdr:to>
@@ -4273,7 +4273,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="18454680"/>
-          <a:ext cx="4491360" cy="526680"/>
+          <a:ext cx="4491000" cy="526680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4326,7 +4326,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>258480</xdr:colOff>
+      <xdr:colOff>258120</xdr:colOff>
       <xdr:row>134</xdr:row>
       <xdr:rowOff>88560</xdr:rowOff>
     </xdr:to>
@@ -4338,7 +4338,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="21684960"/>
-          <a:ext cx="4491360" cy="526680"/>
+          <a:ext cx="4491000" cy="526680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6725,7 +6725,7 @@
   </sheetPr>
   <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -11153,10 +11153,10 @@
   <dimension ref="A1:P46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B36" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
       <selection pane="bottomRight" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -13749,9 +13749,9 @@
   <dimension ref="A1:W11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="X2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topRight" activeCell="X1" activeCellId="0" sqref="X1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
       <selection pane="bottomRight" activeCell="N19" activeCellId="0" sqref="N19"/>
     </sheetView>
@@ -16552,12 +16552,12 @@
   </sheetPr>
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Q4" activeCellId="0" sqref="Q4"/>
+      <selection pane="bottomRight" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>